<commit_message>
feat: complete bulk edit functionality and fix dashboard tests/bugs
</commit_message>
<xml_diff>
--- a/sample_transactions_wrong.xlsx
+++ b/sample_transactions_wrong.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Desktop\HoneyMoney\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Description</t>
   </si>
@@ -54,15 +54,9 @@
     <t>Pablo</t>
   </si>
   <si>
-    <t>2026-01-12</t>
-  </si>
-  <si>
     <t>Weekly Groceries</t>
   </si>
   <si>
-    <t>Groceries</t>
-  </si>
-  <si>
     <t>Expense</t>
   </si>
   <si>
@@ -91,6 +85,15 @@
   </si>
   <si>
     <t>Dateasd</t>
+  </si>
+  <si>
+    <t>as</t>
+  </si>
+  <si>
+    <t>20ddd26-01-12</t>
+  </si>
+  <si>
+    <t>Groceriffes</t>
   </si>
 </sst>
 </file>
@@ -470,14 +473,18 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.625" customWidth="1"/>
+    <col min="2" max="2" width="21.125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -517,56 +524,56 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G3" t="s">
         <v>13</v>
-      </c>
-      <c r="D3">
-        <v>85.5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
       </c>
       <c r="D4">
         <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
       </c>
       <c r="D5">
         <v>500</v>
@@ -581,7 +588,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:E2 B1:E1 G1 A5:E5 G5 A4:G4 A3:E3 G3 G2" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:E2 B1:E1 G1 A5:E5 G5 A4:G4 B3 G3 G2 E3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>